<commit_message>
Update Rizka - Tambahan Cari Mobil Rental 1
</commit_message>
<xml_diff>
--- a/cariMobilRental.xlsx
+++ b/cariMobilRental.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A56C8E-4FDE-4784-8200-FE24C113DF12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71014483-6D6D-4D0B-82AE-1096DD3FB955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{01EB28EE-9F05-4D76-BB58-6F58EBC6F20E}"/>
+    <workbookView xWindow="885" yWindow="0" windowWidth="17895" windowHeight="11070" xr2:uid="{01EB28EE-9F05-4D76-BB58-6F58EBC6F20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>brand</t>
   </si>
@@ -117,6 +117,39 @@
   </si>
   <si>
     <t>Pertanian</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>1.3 VELOZ M/T</t>
+  </si>
+  <si>
+    <t>BINTARO</t>
+  </si>
+  <si>
+    <t>Pribadi</t>
+  </si>
+  <si>
+    <t>PLUIT</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>DAIHATSU</t>
+  </si>
+  <si>
+    <t>AYLA</t>
+  </si>
+  <si>
+    <t>HARAPAN INDAH</t>
+  </si>
+  <si>
+    <t>1.0 D+M/T NEW</t>
+  </si>
+  <si>
+    <t>Finance</t>
   </si>
 </sst>
 </file>
@@ -469,27 +502,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BFA2E6-AED2-41C1-8DDD-DEF406BE1CD8}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -589,6 +626,217 @@
         <v>24</v>
       </c>
     </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>2019</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3">
+        <v>36</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>2019</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4">
+        <v>36</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>2018</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5">
+        <v>24</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6">
+        <v>2018</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6">
+        <v>24</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7">
+        <v>2018</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7">
+        <v>60</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Rizka - Fixing Data Binding Rental Mobil
</commit_message>
<xml_diff>
--- a/cariMobilRental.xlsx
+++ b/cariMobilRental.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2308FE8C-ACBB-4645-AC39-1082E915C503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92019229-810C-435F-B63C-96C433DCBFF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{01EB28EE-9F05-4D76-BB58-6F58EBC6F20E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="47">
   <si>
     <t>brand</t>
   </si>
@@ -72,9 +72,6 @@
     <t>warnaSilver</t>
   </si>
   <si>
-    <t>warnaMerah</t>
-  </si>
-  <si>
     <t>warnaSemua</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Pribadi</t>
   </si>
   <si>
-    <t>PLUIT</t>
-  </si>
-  <si>
     <t>Personal</t>
   </si>
   <si>
@@ -159,9 +153,6 @@
     <t>Used</t>
   </si>
   <si>
-    <t>T:1.0 D+M/T NEW</t>
-  </si>
-  <si>
     <t>DKI Jakarta, Banten, Jawa Barat</t>
   </si>
   <si>
@@ -175,6 +166,15 @@
   </si>
   <si>
     <t>bidangUsahaIsEmptyUsaha</t>
+  </si>
+  <si>
+    <t>AGYA</t>
+  </si>
+  <si>
+    <t>T:1.2 G A/T NEW</t>
+  </si>
+  <si>
+    <t>BANDUNG 3 CIBIRU</t>
   </si>
 </sst>
 </file>
@@ -654,36 +654,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BFA2E6-AED2-41C1-8DDD-DEF406BE1CD8}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
     <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="45.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -730,284 +729,271 @@
       <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="E2" s="6">
         <v>2019</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7">
+      <c r="O2" s="7">
         <v>48</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>24</v>
+      <c r="P2" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E3" s="6">
         <v>2018</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7">
+        <v>36</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E4" s="8">
         <v>2018</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9">
+        <v>22</v>
+      </c>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9">
         <v>36</v>
       </c>
-      <c r="Q4" s="9" t="s">
-        <v>46</v>
+      <c r="P4" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E5" s="8">
         <v>2018</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P5" s="9">
+      <c r="N5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="9">
         <v>24</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="P5" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="D6" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E6" s="8">
         <v>2018</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="H6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P6" s="9">
+      <c r="N6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="9">
         <v>24</v>
       </c>
-      <c r="Q6" s="9" t="s">
-        <v>45</v>
+      <c r="P6" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="E7" s="8">
         <v>2019</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9">
+      <c r="O7" s="9">
         <v>60</v>
       </c>
-      <c r="Q7" s="9" t="s">
-        <v>43</v>
+      <c r="P7" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1036,37 +1022,37 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E1" s="2">
         <v>2019</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L1" s="2">
         <v>12</v>
@@ -1074,37 +1060,37 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="E2" s="4">
         <v>2018</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L2" s="4">
         <v>36</v>
@@ -1112,37 +1098,37 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="E3" s="4">
         <v>2018</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L3" s="4">
         <v>36</v>
@@ -1150,37 +1136,37 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="E4" s="4">
         <v>2018</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L4" s="4">
         <v>36</v>
@@ -1188,37 +1174,37 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="E5" s="4">
         <v>2018</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L5" s="4">
         <v>36</v>
@@ -1226,37 +1212,37 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="E6" s="4">
         <v>2019</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="H6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="K6" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L6" s="4">
         <v>60</v>

</xml_diff>